<commit_message>
Self Service price sheet enhancement
</commit_message>
<xml_diff>
--- a/CostPriceSheetTemplate.xlsx
+++ b/CostPriceSheetTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\IdeaProjects\qa-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF75693-A86E-43EE-82E2-A228306AC6CB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1629A49-625C-4C13-82F7-18FDF6222A79}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1260,7 +1260,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1327,13 +1327,13 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>7.5</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>10</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1356,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>10</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1379,7 +1379,7 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>10</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>